<commit_message>
give players joining through sockets a human player behaviour
</commit_message>
<xml_diff>
--- a/Docs/correction_grid.xlsx
+++ b/Docs/correction_grid.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\Quest\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21D3AAF-1BBE-4AEB-A32B-A1C2698054DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31240" windowHeight="22480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="179017" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -608,7 +614,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1267,6 +1273,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1591,22 +1605,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="80.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.125" customWidth="1"/>
+    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>113</v>
       </c>
@@ -1614,7 +1628,7 @@
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>115</v>
       </c>
@@ -1622,29 +1636,33 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3">
+        <v>57</v>
+      </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
@@ -1652,7 +1670,7 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
@@ -1660,18 +1678,18 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
@@ -1679,7 +1697,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="7"/>
@@ -1692,7 +1710,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -1702,7 +1720,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>22</v>
       </c>
@@ -1712,7 +1730,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>23</v>
       </c>
@@ -1722,7 +1740,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>26</v>
       </c>
@@ -1732,7 +1750,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>24</v>
       </c>
@@ -1742,7 +1760,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>25</v>
       </c>
@@ -1752,13 +1770,13 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="9"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="7" t="s">
         <v>6</v>
@@ -1777,7 +1795,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
@@ -1785,17 +1803,19 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="5"/>
+      <c r="B21" s="5">
+        <v>5</v>
+      </c>
       <c r="C21">
         <v>5</v>
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>114</v>
       </c>
@@ -1804,7 +1824,7 @@
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>18</v>
       </c>
@@ -1814,57 +1834,57 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>105</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>106</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>107</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>64</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>28</v>
       </c>
@@ -1874,7 +1894,7 @@
       </c>
       <c r="D32" s="7"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>30</v>
       </c>
@@ -1883,7 +1903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>31</v>
       </c>
@@ -1892,7 +1912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>32</v>
       </c>
@@ -1901,7 +1921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>33</v>
       </c>
@@ -1910,7 +1930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>34</v>
       </c>
@@ -1919,7 +1939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>38</v>
       </c>
@@ -1928,13 +1948,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C39" s="7"/>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>40</v>
       </c>
@@ -1943,14 +1963,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>35</v>
       </c>
@@ -1959,7 +1979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>41</v>
       </c>
@@ -1968,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>42</v>
       </c>
@@ -1977,7 +1997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>36</v>
       </c>
@@ -1986,7 +2006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>43</v>
       </c>
@@ -1995,7 +2015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>44</v>
       </c>
@@ -2004,7 +2024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>45</v>
       </c>
@@ -2013,13 +2033,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>46</v>
       </c>
       <c r="C49" s="7"/>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>47</v>
       </c>
@@ -2028,7 +2048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>48</v>
       </c>
@@ -2037,7 +2057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>50</v>
       </c>
@@ -2046,7 +2066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>51</v>
       </c>
@@ -2055,7 +2075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>52</v>
       </c>
@@ -2064,7 +2084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>79</v>
       </c>
@@ -2073,7 +2093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>49</v>
       </c>
@@ -2082,7 +2102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>53</v>
       </c>
@@ -2091,7 +2111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>54</v>
       </c>
@@ -2100,13 +2120,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C59" s="7"/>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>56</v>
       </c>
@@ -2115,7 +2135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>57</v>
       </c>
@@ -2124,7 +2144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>58</v>
       </c>
@@ -2133,7 +2153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>65</v>
       </c>
@@ -2142,7 +2162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>66</v>
       </c>
@@ -2151,27 +2171,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="C65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="C66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>59</v>
       </c>
       <c r="C67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>61</v>
       </c>
@@ -2180,7 +2200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>62</v>
       </c>
@@ -2190,7 +2210,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>63</v>
       </c>
@@ -2199,18 +2219,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C72" s="7"/>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>67</v>
       </c>
       <c r="C73" s="7"/>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>68</v>
       </c>
@@ -2219,7 +2239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>69</v>
       </c>
@@ -2229,7 +2249,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>70</v>
       </c>
@@ -2238,7 +2258,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>71</v>
       </c>
@@ -2248,14 +2268,14 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C78" s="7"/>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>73</v>
       </c>
@@ -2265,7 +2285,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>74</v>
       </c>
@@ -2275,7 +2295,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>75</v>
       </c>
@@ -2285,7 +2305,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>76</v>
       </c>
@@ -2295,7 +2315,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>77</v>
       </c>
@@ -2305,12 +2325,12 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="7"/>
       <c r="C84" s="7"/>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>80</v>
       </c>
@@ -2323,19 +2343,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="7"/>
       <c r="C86" s="7"/>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>112</v>
       </c>
       <c r="C87" s="7"/>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>108</v>
       </c>
@@ -2345,7 +2365,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>109</v>
       </c>
@@ -2355,7 +2375,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>110</v>
       </c>
@@ -2365,7 +2385,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>111</v>
       </c>
@@ -2375,7 +2395,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>4</v>
       </c>
@@ -2385,7 +2405,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>5</v>
       </c>
@@ -2395,7 +2415,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>8</v>
       </c>
@@ -2405,7 +2425,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>7</v>
       </c>
@@ -2415,7 +2435,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>0</v>
       </c>
@@ -2425,7 +2445,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>9</v>
       </c>
@@ -2434,7 +2454,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>1</v>
       </c>
@@ -2443,7 +2463,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>3</v>
       </c>
@@ -2452,7 +2472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>102</v>
       </c>
@@ -2461,7 +2481,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>103</v>
       </c>
@@ -2470,7 +2490,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>88</v>
       </c>
@@ -2479,7 +2499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>82</v>
       </c>
@@ -2488,7 +2508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>83</v>
       </c>
@@ -2497,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>84</v>
       </c>
@@ -2506,7 +2526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>85</v>
       </c>
@@ -2515,7 +2535,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>86</v>
       </c>
@@ -2524,7 +2544,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
         <v>87</v>
       </c>
@@ -2533,7 +2553,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>89</v>
       </c>
@@ -2543,7 +2563,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>90</v>
       </c>
@@ -2553,7 +2573,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>91</v>
       </c>
@@ -2563,7 +2583,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>92</v>
       </c>
@@ -2573,7 +2593,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>93</v>
       </c>
@@ -2583,7 +2603,7 @@
       </c>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>94</v>
       </c>
@@ -2593,7 +2613,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>95</v>
       </c>
@@ -2602,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
         <v>96</v>
       </c>
@@ -2611,7 +2631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>97</v>
       </c>
@@ -2620,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
         <v>98</v>
       </c>
@@ -2629,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>99</v>
       </c>
@@ -2638,7 +2658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E120" t="s">
         <v>119</v>
       </c>
@@ -2647,12 +2667,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>104</v>
       </c>
@@ -2661,7 +2681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>123</v>
       </c>
@@ -2670,7 +2690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>120</v>
       </c>
@@ -2679,7 +2699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>121</v>
       </c>
@@ -2688,7 +2708,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>122</v>
       </c>
@@ -2697,7 +2717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>117</v>
       </c>
@@ -2706,7 +2726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E128" t="s">
         <v>101</v>
       </c>
@@ -2715,12 +2735,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>116</v>
       </c>
@@ -2729,11 +2749,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B131" s="11"/>
+      <c r="B131" s="11">
+        <v>2</v>
+      </c>
       <c r="C131">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
added update player area after discard
</commit_message>
<xml_diff>
--- a/Docs/correction_grid.xlsx
+++ b/Docs/correction_grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\Quest\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21D3AAF-1BBE-4AEB-A32B-A1C2698054DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E59E29A-C25A-4743-ABFD-FD65B11A3B9B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="128">
   <si>
     <t>is it possible for a participant to NOT play a card for a stage</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -609,6 +609,15 @@
   </si>
   <si>
     <t>use of JSON</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>tbd</t>
+  </si>
+  <si>
+    <t>Claimed Total</t>
   </si>
 </sst>
 </file>
@@ -1606,10 +1615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1828,7 +1837,9 @@
       <c r="A23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="5">
+        <v>5</v>
+      </c>
       <c r="C23" s="7">
         <v>5</v>
       </c>
@@ -1888,7 +1899,9 @@
       <c r="A32" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="5"/>
+      <c r="B32" s="5">
+        <v>1</v>
+      </c>
       <c r="C32" s="7">
         <v>1</v>
       </c>
@@ -1898,7 +1911,9 @@
       <c r="A33" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="5"/>
+      <c r="B33" s="5">
+        <v>1</v>
+      </c>
       <c r="C33" s="7">
         <v>1</v>
       </c>
@@ -1907,7 +1922,9 @@
       <c r="A34" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="5"/>
+      <c r="B34" s="5">
+        <v>1</v>
+      </c>
       <c r="C34" s="7">
         <v>1</v>
       </c>
@@ -1916,7 +1933,9 @@
       <c r="A35" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="5"/>
+      <c r="B35" s="5">
+        <v>1</v>
+      </c>
       <c r="C35" s="7">
         <v>1</v>
       </c>
@@ -1925,7 +1944,9 @@
       <c r="A36" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="5"/>
+      <c r="B36" s="5">
+        <v>1</v>
+      </c>
       <c r="C36" s="7">
         <v>1</v>
       </c>
@@ -2028,7 +2049,9 @@
       <c r="A48" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="5"/>
+      <c r="B48" s="5">
+        <v>2</v>
+      </c>
       <c r="C48" s="7">
         <v>2</v>
       </c>
@@ -2043,7 +2066,9 @@
       <c r="A50" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="5"/>
+      <c r="B50" s="5">
+        <v>1</v>
+      </c>
       <c r="C50" s="7">
         <v>1</v>
       </c>
@@ -2052,7 +2077,9 @@
       <c r="A51" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="5"/>
+      <c r="B51" s="5" t="s">
+        <v>125</v>
+      </c>
       <c r="C51" s="7">
         <v>1</v>
       </c>
@@ -2106,7 +2133,9 @@
       <c r="A57" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B57" s="11"/>
+      <c r="B57" s="11">
+        <v>1</v>
+      </c>
       <c r="C57" s="7">
         <v>1</v>
       </c>
@@ -2148,7 +2177,9 @@
       <c r="A62" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B62" s="11"/>
+      <c r="B62" s="11">
+        <v>1</v>
+      </c>
       <c r="C62" s="7">
         <v>1</v>
       </c>
@@ -2157,7 +2188,9 @@
       <c r="A63" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B63" s="11"/>
+      <c r="B63" s="11">
+        <v>1</v>
+      </c>
       <c r="C63" s="7">
         <v>1</v>
       </c>
@@ -2166,7 +2199,9 @@
       <c r="A64" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B64" s="11"/>
+      <c r="B64" s="11">
+        <v>1</v>
+      </c>
       <c r="C64" s="7">
         <v>1</v>
       </c>
@@ -2409,7 +2444,9 @@
       <c r="A93" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B93" s="11"/>
+      <c r="B93" s="11">
+        <v>0.5</v>
+      </c>
       <c r="C93">
         <v>0.5</v>
       </c>
@@ -2419,7 +2456,9 @@
       <c r="A94" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B94" s="11"/>
+      <c r="B94" s="11">
+        <v>0.5</v>
+      </c>
       <c r="C94">
         <v>0.5</v>
       </c>
@@ -2429,7 +2468,9 @@
       <c r="A95" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B95" s="11"/>
+      <c r="B95" s="11">
+        <v>0.5</v>
+      </c>
       <c r="C95">
         <v>0.5</v>
       </c>
@@ -2439,7 +2480,9 @@
       <c r="A96" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B96" s="11"/>
+      <c r="B96" s="11">
+        <v>0.5</v>
+      </c>
       <c r="C96" s="7">
         <v>0.5</v>
       </c>
@@ -2449,25 +2492,37 @@
       <c r="A97" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B97" s="11"/>
+      <c r="B97" s="11">
+        <v>0.5</v>
+      </c>
       <c r="C97" s="7">
         <v>0.5</v>
       </c>
+      <c r="D97" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B98" s="11"/>
+      <c r="B98" s="11">
+        <v>0.5</v>
+      </c>
       <c r="C98" s="7">
         <v>0.5</v>
+      </c>
+      <c r="D98" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B99" s="11"/>
+      <c r="B99" s="11">
+        <v>1</v>
+      </c>
       <c r="C99" s="7">
         <v>1</v>
       </c>
@@ -2476,7 +2531,9 @@
       <c r="A100" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B100" s="11"/>
+      <c r="B100" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="C100" s="7">
         <v>0.5</v>
       </c>
@@ -2485,7 +2542,9 @@
       <c r="A101" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B101" s="11"/>
+      <c r="B101" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="C101" s="7">
         <v>0.5</v>
       </c>
@@ -2494,25 +2553,37 @@
       <c r="A102" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B102" s="11"/>
+      <c r="B102" s="11">
+        <v>1</v>
+      </c>
       <c r="C102" s="7">
         <v>1</v>
+      </c>
+      <c r="D102" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B103" s="11"/>
+      <c r="B103" s="11">
+        <v>1</v>
+      </c>
       <c r="C103" s="7">
         <v>1</v>
+      </c>
+      <c r="D103" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B104" s="11"/>
+      <c r="B104" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="C104" s="7">
         <v>1</v>
       </c>
@@ -2521,25 +2592,37 @@
       <c r="A105" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B105" s="11"/>
+      <c r="B105" s="11">
+        <v>1</v>
+      </c>
       <c r="C105" s="7">
         <v>1</v>
+      </c>
+      <c r="D105" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B106" s="11"/>
+      <c r="B106" s="11">
+        <v>0.5</v>
+      </c>
       <c r="C106" s="7">
         <v>0.5</v>
+      </c>
+      <c r="D106" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B107" s="11"/>
+      <c r="B107" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="C107" s="7">
         <v>0.5</v>
       </c>
@@ -2557,7 +2640,9 @@
       <c r="A109" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B109" s="11"/>
+      <c r="B109" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="C109" s="7">
         <v>1</v>
       </c>
@@ -2567,9 +2652,14 @@
       <c r="A110" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B110" s="11"/>
+      <c r="B110" s="11">
+        <v>1</v>
+      </c>
       <c r="C110" s="7">
         <v>1</v>
+      </c>
+      <c r="D110" t="s">
+        <v>126</v>
       </c>
       <c r="E110" s="7"/>
     </row>
@@ -2577,9 +2667,14 @@
       <c r="A111" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B111" s="11"/>
+      <c r="B111" s="11">
+        <v>0.5</v>
+      </c>
       <c r="C111" s="7">
         <v>0.5</v>
+      </c>
+      <c r="D111" t="s">
+        <v>126</v>
       </c>
       <c r="E111" s="7"/>
     </row>
@@ -2587,7 +2682,9 @@
       <c r="A112" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B112" s="11"/>
+      <c r="B112" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="C112" s="7">
         <v>2</v>
       </c>
@@ -2597,7 +2694,9 @@
       <c r="A113" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B113" s="11"/>
+      <c r="B113" s="11">
+        <v>0</v>
+      </c>
       <c r="C113" s="7">
         <v>1.5</v>
       </c>
@@ -2607,9 +2706,14 @@
       <c r="A114" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B114" s="11"/>
+      <c r="B114" s="11">
+        <v>1</v>
+      </c>
       <c r="C114" s="7">
         <v>1</v>
+      </c>
+      <c r="D114" t="s">
+        <v>126</v>
       </c>
       <c r="E114" s="7"/>
     </row>
@@ -2617,16 +2721,23 @@
       <c r="A115" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B115" s="11"/>
+      <c r="B115" s="11">
+        <v>1</v>
+      </c>
       <c r="C115" s="7">
         <v>1</v>
+      </c>
+      <c r="D115" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B116" s="11"/>
+      <c r="B116" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="C116" s="7">
         <v>1</v>
       </c>
@@ -2635,7 +2746,9 @@
       <c r="A117" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B117" s="11"/>
+      <c r="B117" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="C117" s="7">
         <v>1</v>
       </c>
@@ -2644,18 +2757,28 @@
       <c r="A118" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B118" s="11"/>
+      <c r="B118" s="11">
+        <v>1</v>
+      </c>
       <c r="C118" s="7">
         <v>1</v>
+      </c>
+      <c r="D118" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B119" s="11"/>
+      <c r="B119" s="11">
+        <v>1</v>
+      </c>
       <c r="C119" s="7">
         <v>1</v>
+      </c>
+      <c r="D119" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -2694,7 +2817,9 @@
       <c r="A124" t="s">
         <v>120</v>
       </c>
-      <c r="B124" s="11"/>
+      <c r="B124" s="11">
+        <v>0</v>
+      </c>
       <c r="C124">
         <v>2</v>
       </c>
@@ -2758,6 +2883,19 @@
       </c>
       <c r="C131">
         <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>127</v>
+      </c>
+      <c r="B134">
+        <f>SUM(B32:B131)</f>
+        <v>27</v>
+      </c>
+      <c r="C134">
+        <f>B134/(100-8)</f>
+        <v>0.29347826086956524</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added confirm cards event to server
</commit_message>
<xml_diff>
--- a/Docs/correction_grid.xlsx
+++ b/Docs/correction_grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\Quest\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E59E29A-C25A-4743-ABFD-FD65B11A3B9B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8377659D-E96B-4EAA-BB43-60185A0A4828}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1617,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D136" sqref="D136"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
log info for scenario 1 correction grid
</commit_message>
<xml_diff>
--- a/Docs/correction_grid.xlsx
+++ b/Docs/correction_grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\Quest\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8377659D-E96B-4EAA-BB43-60185A0A4828}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B0D487-C82E-484F-A4E6-F340589CF86B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="157">
   <si>
     <t>is it possible for a participant to NOT play a card for a stage</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -611,13 +611,100 @@
     <t>use of JSON</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>tbd</t>
   </si>
   <si>
     <t>Claimed Total</t>
+  </si>
+  <si>
+    <t>s1e.log[9687-9693]</t>
+  </si>
+  <si>
+    <t>s1.log[61], s1e.log[9850-9879]</t>
+  </si>
+  <si>
+    <t>s1.log[60], s1e.log[9627-9686]</t>
+  </si>
+  <si>
+    <t>s1e.log[239-394]</t>
+  </si>
+  <si>
+    <t>s1.log[1-58], s1e.log[1-30]</t>
+  </si>
+  <si>
+    <t>s1.log[62], s1e.log[9880-10121]</t>
+  </si>
+  <si>
+    <t>s1.log[63]</t>
+  </si>
+  <si>
+    <t>s1e.log[10367-10373]</t>
+  </si>
+  <si>
+    <t>s1.log[64], s1e.log[10381-10386]</t>
+  </si>
+  <si>
+    <t>s1e.log[10387-10410]</t>
+  </si>
+  <si>
+    <t>s1e.log[10626-10631]</t>
+  </si>
+  <si>
+    <t>s1.log[65], s1e.log[10633-10721]</t>
+  </si>
+  <si>
+    <t>s1e.log[10722-10877]</t>
+  </si>
+  <si>
+    <t>s1e.log[10878-10884]</t>
+  </si>
+  <si>
+    <t>s1.log[66], s1e.log[10885-10973]</t>
+  </si>
+  <si>
+    <t>s1e.log[11013-11129]</t>
+  </si>
+  <si>
+    <t>s1.log[67-69]</t>
+  </si>
+  <si>
+    <t>s1e.log[11130-11141]</t>
+  </si>
+  <si>
+    <t>s1.log[73], s1e.log[13815-13838]</t>
+  </si>
+  <si>
+    <t>s1e.log[14741-14959]</t>
+  </si>
+  <si>
+    <t>s1.log[74-75]</t>
+  </si>
+  <si>
+    <t>s1.log[70-72], s1e.log[14741-14959]</t>
+  </si>
+  <si>
+    <t>validated server side</t>
+  </si>
+  <si>
+    <t>s1e.log[15023-15178]</t>
+  </si>
+  <si>
+    <t>s1.log[78-84]</t>
+  </si>
+  <si>
+    <t>s1.log[90-92]</t>
+  </si>
+  <si>
+    <t>s1.log[93-96]</t>
+  </si>
+  <si>
+    <t>s1e.log[20645-20836]</t>
+  </si>
+  <si>
+    <t>s1.log[100-112], s1e.log[21866-21921]</t>
+  </si>
+  <si>
+    <t>s1.log[114-125]</t>
   </si>
 </sst>
 </file>
@@ -989,13 +1076,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1003,7 +1088,27 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="273">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1617,100 +1722,100 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="80.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="11" customWidth="1"/>
     <col min="3" max="3" width="6.125" customWidth="1"/>
-    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="10">
         <v>57</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="10">
         <v>4</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="E9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
       <c r="E11" t="s">
         <v>29</v>
       </c>
@@ -1720,83 +1825,83 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="12"/>
+      <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="7">
-        <v>1</v>
-      </c>
-      <c r="D13" s="7"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="7">
+      <c r="B14" s="12"/>
+      <c r="C14" s="5">
         <v>2</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="7">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="7">
+      <c r="B16" s="12"/>
+      <c r="C16" s="5">
         <v>2</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="7">
+      <c r="B17" s="12"/>
+      <c r="C17" s="5">
         <v>2</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="7" t="s">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="5" t="s">
         <v>78</v>
       </c>
       <c r="F19">
@@ -1805,572 +1910,693 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="14">
         <v>5</v>
       </c>
       <c r="C21">
         <v>5</v>
       </c>
-      <c r="D21" s="7"/>
+      <c r="D21" s="5" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="14">
         <v>5</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="5">
         <v>5</v>
       </c>
-      <c r="D23" s="7"/>
+      <c r="D23" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="A28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="7"/>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="5">
-        <v>1</v>
-      </c>
-      <c r="C32" s="7">
-        <v>1</v>
-      </c>
-      <c r="D32" s="7"/>
+      <c r="B32" s="14">
+        <v>1</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="5">
-        <v>1</v>
-      </c>
-      <c r="C33" s="7">
-        <v>1</v>
+      <c r="B33" s="14">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="5">
-        <v>1</v>
-      </c>
-      <c r="C34" s="7">
-        <v>1</v>
+      <c r="B34" s="14">
+        <v>1</v>
+      </c>
+      <c r="C34" s="5">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="5">
-        <v>1</v>
-      </c>
-      <c r="C35" s="7">
-        <v>1</v>
+      <c r="B35" s="14">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="5">
-        <v>1</v>
-      </c>
-      <c r="C36" s="7">
-        <v>1</v>
+      <c r="B36" s="14">
+        <v>1</v>
+      </c>
+      <c r="C36" s="5">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="7">
-        <v>1</v>
+      <c r="B37" s="14">
+        <v>1</v>
+      </c>
+      <c r="C37" s="5">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="7">
-        <v>1</v>
+      <c r="B38" s="14">
+        <v>1</v>
+      </c>
+      <c r="C38" s="5">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="7"/>
+      <c r="C39" s="5"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="7">
-        <v>1</v>
+      <c r="B40" s="14">
+        <v>1</v>
+      </c>
+      <c r="C40" s="5">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="7">
-        <v>1</v>
+      <c r="B42" s="14">
+        <v>1</v>
+      </c>
+      <c r="C42" s="5">
+        <v>1</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="7">
-        <v>1</v>
+      <c r="B43" s="14">
+        <v>1</v>
+      </c>
+      <c r="C43" s="5">
+        <v>1</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="7">
-        <v>1</v>
+      <c r="B44" s="14">
+        <v>1</v>
+      </c>
+      <c r="C44" s="5">
+        <v>1</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="7">
-        <v>1</v>
+      <c r="B45" s="14">
+        <v>1</v>
+      </c>
+      <c r="C45" s="5">
+        <v>1</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="7">
-        <v>1</v>
+      <c r="B46" s="14">
+        <v>1</v>
+      </c>
+      <c r="C46" s="5">
+        <v>1</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="7">
-        <v>1</v>
+      <c r="B47" s="14">
+        <v>1</v>
+      </c>
+      <c r="C47" s="5">
+        <v>1</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48" s="14">
         <v>2</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+      <c r="D48" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="7"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
+      <c r="C49" s="5"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="5">
-        <v>1</v>
-      </c>
-      <c r="C50" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
+      <c r="B50" s="14">
+        <v>1</v>
+      </c>
+      <c r="C50" s="5">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C51" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
+      <c r="B51" s="14">
+        <v>1</v>
+      </c>
+      <c r="C51" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
+      <c r="B52" s="14">
+        <v>1</v>
+      </c>
+      <c r="C52" s="5">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
+      <c r="B53" s="14">
+        <v>1</v>
+      </c>
+      <c r="C53" s="5">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
+      <c r="B54" s="14">
+        <v>1</v>
+      </c>
+      <c r="C54" s="5">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
+      <c r="B55" s="15">
+        <v>1</v>
+      </c>
+      <c r="C55" s="5">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B56" s="11"/>
-      <c r="C56" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+      <c r="B56" s="15">
+        <v>1</v>
+      </c>
+      <c r="C56" s="5">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B57" s="11">
-        <v>1</v>
-      </c>
-      <c r="C57" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
+      <c r="B57" s="15">
+        <v>1</v>
+      </c>
+      <c r="C57" s="5">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="11"/>
-      <c r="C58" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
+      <c r="B58" s="15">
+        <v>1</v>
+      </c>
+      <c r="C58" s="5">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C59" s="7"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
+      <c r="C59" s="5"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B60" s="11"/>
-      <c r="C60" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
+      <c r="B60" s="15">
+        <v>1</v>
+      </c>
+      <c r="C60" s="5">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B61" s="11"/>
-      <c r="C61" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
+      <c r="B61" s="15">
+        <v>1</v>
+      </c>
+      <c r="C61" s="5">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B62" s="11">
-        <v>1</v>
-      </c>
-      <c r="C62" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
+      <c r="B62" s="15">
+        <v>1</v>
+      </c>
+      <c r="C62" s="5">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B63" s="11">
-        <v>1</v>
-      </c>
-      <c r="C63" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
+      <c r="B63" s="15">
+        <v>1</v>
+      </c>
+      <c r="C63" s="5">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B64" s="11">
-        <v>1</v>
-      </c>
-      <c r="C64" s="7">
-        <v>1</v>
+      <c r="B64" s="15">
+        <v>1</v>
+      </c>
+      <c r="C64" s="5">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
-      <c r="C65" s="7"/>
+      <c r="A65" s="5"/>
+      <c r="C65" s="5"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="7"/>
-      <c r="C66" s="7"/>
+      <c r="A66" s="5"/>
+      <c r="C66" s="5"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C67" s="7"/>
+      <c r="C67" s="5"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
+      <c r="A68" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C68" s="7"/>
+      <c r="C68" s="5"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
+      <c r="A69" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B69" s="11"/>
-      <c r="C69" s="7">
+      <c r="B69" s="15"/>
+      <c r="C69" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B70" s="11"/>
-      <c r="C70" s="7">
+      <c r="B70" s="15"/>
+      <c r="C70" s="5">
         <v>2</v>
       </c>
-      <c r="E70" s="7"/>
+      <c r="E70" s="5"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
+      <c r="A71" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="7">
+      <c r="B71" s="15"/>
+      <c r="C71" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C72" s="7"/>
-      <c r="E72" s="7"/>
+      <c r="C72" s="5"/>
+      <c r="E72" s="5"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>67</v>
       </c>
-      <c r="C73" s="7"/>
-      <c r="E73" s="7"/>
+      <c r="C73" s="5"/>
+      <c r="E73" s="5"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B74" s="11"/>
-      <c r="C74" s="7">
+      <c r="B74" s="15"/>
+      <c r="C74" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B75" s="11"/>
-      <c r="C75" s="7">
-        <v>1</v>
-      </c>
-      <c r="E75" s="7"/>
+      <c r="B75" s="15"/>
+      <c r="C75" s="5">
+        <v>1</v>
+      </c>
+      <c r="E75" s="5"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
+      <c r="A76" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C76" s="7">
+      <c r="C76" s="5">
         <v>0.5</v>
       </c>
-      <c r="E76" s="7"/>
+      <c r="E76" s="5"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B77" s="11"/>
-      <c r="C77" s="7">
+      <c r="B77" s="15"/>
+      <c r="C77" s="5">
         <v>0.5</v>
       </c>
-      <c r="E77" s="7"/>
+      <c r="E77" s="5"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C78" s="7"/>
-      <c r="E78" s="7"/>
+      <c r="C78" s="5"/>
+      <c r="E78" s="5"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
+      <c r="A79" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B79" s="11"/>
-      <c r="C79" s="7">
+      <c r="B79" s="15"/>
+      <c r="C79" s="5">
         <v>2</v>
       </c>
-      <c r="E79" s="7"/>
+      <c r="E79" s="5"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="7" t="s">
+      <c r="A80" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B80" s="11"/>
-      <c r="C80" s="7">
-        <v>1</v>
-      </c>
-      <c r="E80" s="7"/>
+      <c r="B80" s="15"/>
+      <c r="C80" s="5">
+        <v>1</v>
+      </c>
+      <c r="E80" s="5"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B81" s="11"/>
-      <c r="C81" s="7">
-        <v>1</v>
-      </c>
-      <c r="E81" s="7"/>
+      <c r="B81" s="15"/>
+      <c r="C81" s="5">
+        <v>1</v>
+      </c>
+      <c r="E81" s="5"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B82" s="11"/>
-      <c r="C82" s="7">
-        <v>1</v>
-      </c>
-      <c r="E82" s="7"/>
+      <c r="B82" s="15"/>
+      <c r="C82" s="5">
+        <v>1</v>
+      </c>
+      <c r="E82" s="5"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="7" t="s">
+      <c r="A83" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B83" s="11"/>
-      <c r="C83" s="7">
-        <v>1</v>
-      </c>
-      <c r="E83" s="7"/>
+      <c r="B83" s="15"/>
+      <c r="C83" s="5">
+        <v>1</v>
+      </c>
+      <c r="E83" s="5"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="7"/>
-      <c r="C84" s="7"/>
-      <c r="E84" s="7"/>
+      <c r="A84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="E84" s="5"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="6" t="s">
+      <c r="A85" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C85" s="7"/>
-      <c r="E85" s="7" t="s">
+      <c r="C85" s="5"/>
+      <c r="E85" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F85">
@@ -2379,406 +2605,354 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="7"/>
-      <c r="C86" s="7"/>
-      <c r="E86" s="7"/>
+      <c r="A86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="E86" s="5"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="7" t="s">
+      <c r="A87" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C87" s="7"/>
-      <c r="E87" s="7"/>
+      <c r="C87" s="5"/>
+      <c r="E87" s="5"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="7">
-        <v>1</v>
-      </c>
-      <c r="E88" s="7"/>
+      <c r="B88" s="15"/>
+      <c r="C88" s="5">
+        <v>1</v>
+      </c>
+      <c r="E88" s="5"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="7" t="s">
+      <c r="A89" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B89" s="11"/>
-      <c r="C89" s="7">
-        <v>1</v>
-      </c>
-      <c r="E89" s="7"/>
+      <c r="B89" s="15"/>
+      <c r="C89" s="5">
+        <v>1</v>
+      </c>
+      <c r="E89" s="5"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="7" t="s">
+      <c r="A90" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B90" s="11"/>
-      <c r="C90" s="7">
-        <v>1</v>
-      </c>
-      <c r="E90" s="7"/>
+      <c r="B90" s="15"/>
+      <c r="C90" s="5">
+        <v>1</v>
+      </c>
+      <c r="E90" s="5"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="7" t="s">
+      <c r="A91" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B91" s="11"/>
-      <c r="C91" s="7">
-        <v>1</v>
-      </c>
-      <c r="E91" s="7"/>
+      <c r="B91" s="15"/>
+      <c r="C91" s="5">
+        <v>1</v>
+      </c>
+      <c r="E91" s="5"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="7" t="s">
+      <c r="A92" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B92" s="11"/>
+      <c r="B92" s="15"/>
       <c r="C92">
         <v>0.5</v>
       </c>
-      <c r="E92" s="7"/>
+      <c r="E92" s="5"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="4" t="s">
+      <c r="A93" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B93" s="11">
-        <v>0.5</v>
-      </c>
+      <c r="B93" s="15"/>
       <c r="C93">
         <v>0.5</v>
       </c>
-      <c r="E93" s="7"/>
+      <c r="E93" s="5"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="7" t="s">
+      <c r="A94" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B94" s="11">
-        <v>0.5</v>
-      </c>
+      <c r="B94" s="15"/>
       <c r="C94">
         <v>0.5</v>
       </c>
-      <c r="E94" s="7"/>
+      <c r="E94" s="5"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="7" t="s">
+      <c r="A95" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B95" s="11">
-        <v>0.5</v>
-      </c>
+      <c r="B95" s="15"/>
       <c r="C95">
         <v>0.5</v>
       </c>
-      <c r="E95" s="7"/>
+      <c r="E95" s="5"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="7" t="s">
+      <c r="A96" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B96" s="11">
+      <c r="B96" s="15"/>
+      <c r="C96" s="5">
         <v>0.5</v>
       </c>
-      <c r="C96" s="7">
+      <c r="E96" s="5"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B97" s="15"/>
+      <c r="C97" s="5">
         <v>0.5</v>
       </c>
-      <c r="E96" s="7"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B97" s="11">
+      <c r="D97" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B98" s="15"/>
+      <c r="C98" s="5">
         <v>0.5</v>
       </c>
-      <c r="C97" s="7">
+      <c r="D98" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B99" s="15"/>
+      <c r="C99" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B100" s="15"/>
+      <c r="C100" s="5">
         <v>0.5</v>
       </c>
-      <c r="D97" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B98" s="11">
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B101" s="15"/>
+      <c r="C101" s="5">
         <v>0.5</v>
       </c>
-      <c r="C98" s="7">
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B102" s="15"/>
+      <c r="C102" s="5">
+        <v>1</v>
+      </c>
+      <c r="D102" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B103" s="15"/>
+      <c r="C103" s="5">
+        <v>1</v>
+      </c>
+      <c r="D103" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B104" s="15"/>
+      <c r="C104" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B105" s="15"/>
+      <c r="C105" s="5">
+        <v>1</v>
+      </c>
+      <c r="D105" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B106" s="15"/>
+      <c r="C106" s="5">
         <v>0.5</v>
       </c>
-      <c r="D98" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B99" s="11">
-        <v>1</v>
-      </c>
-      <c r="C99" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B100" s="11" t="s">
+      <c r="D106" t="s">
         <v>125</v>
       </c>
-      <c r="C100" s="7">
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B107" s="15"/>
+      <c r="C107" s="5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B101" s="11" t="s">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B108" s="15"/>
+      <c r="C108" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B109" s="15"/>
+      <c r="C109" s="5">
+        <v>1</v>
+      </c>
+      <c r="E109" s="5"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B110" s="15"/>
+      <c r="C110" s="5">
+        <v>1</v>
+      </c>
+      <c r="D110" t="s">
         <v>125</v>
       </c>
-      <c r="C101" s="7">
+      <c r="E110" s="5"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B111" s="15"/>
+      <c r="C111" s="5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B102" s="11">
-        <v>1</v>
-      </c>
-      <c r="C102" s="7">
-        <v>1</v>
-      </c>
-      <c r="D102" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B103" s="11">
-        <v>1</v>
-      </c>
-      <c r="C103" s="7">
-        <v>1</v>
-      </c>
-      <c r="D103" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B104" s="11" t="s">
+      <c r="D111" t="s">
         <v>125</v>
       </c>
-      <c r="C104" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B105" s="11">
-        <v>1</v>
-      </c>
-      <c r="C105" s="7">
-        <v>1</v>
-      </c>
-      <c r="D105" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B106" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="C106" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="D106" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B107" s="11" t="s">
+      <c r="E111" s="5"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B112" s="15"/>
+      <c r="C112" s="5">
+        <v>2</v>
+      </c>
+      <c r="E112" s="5"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B113" s="15"/>
+      <c r="C113" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="E113" s="5"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B114" s="15"/>
+      <c r="C114" s="5">
+        <v>1</v>
+      </c>
+      <c r="D114" t="s">
         <v>125</v>
       </c>
-      <c r="C107" s="7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B108" s="11"/>
-      <c r="C108" s="7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B109" s="11" t="s">
+      <c r="E114" s="5"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B115" s="15"/>
+      <c r="C115" s="5">
+        <v>1</v>
+      </c>
+      <c r="D115" t="s">
         <v>125</v>
       </c>
-      <c r="C109" s="7">
-        <v>1</v>
-      </c>
-      <c r="E109" s="7"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B110" s="11">
-        <v>1</v>
-      </c>
-      <c r="C110" s="7">
-        <v>1</v>
-      </c>
-      <c r="D110" t="s">
-        <v>126</v>
-      </c>
-      <c r="E110" s="7"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B111" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="C111" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="D111" t="s">
-        <v>126</v>
-      </c>
-      <c r="E111" s="7"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B112" s="11" t="s">
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B116" s="15"/>
+      <c r="C116" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B117" s="15"/>
+      <c r="C117" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B118" s="15"/>
+      <c r="C118" s="5">
+        <v>1</v>
+      </c>
+      <c r="D118" t="s">
         <v>125</v>
       </c>
-      <c r="C112" s="7">
-        <v>2</v>
-      </c>
-      <c r="E112" s="7"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B113" s="11">
-        <v>0</v>
-      </c>
-      <c r="C113" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="E113" s="7"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B114" s="11">
-        <v>1</v>
-      </c>
-      <c r="C114" s="7">
-        <v>1</v>
-      </c>
-      <c r="D114" t="s">
-        <v>126</v>
-      </c>
-      <c r="E114" s="7"/>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B115" s="11">
-        <v>1</v>
-      </c>
-      <c r="C115" s="7">
-        <v>1</v>
-      </c>
-      <c r="D115" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B116" s="11" t="s">
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B119" s="15"/>
+      <c r="C119" s="5">
+        <v>1</v>
+      </c>
+      <c r="D119" t="s">
         <v>125</v>
-      </c>
-      <c r="C116" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B117" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C117" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B118" s="11">
-        <v>1</v>
-      </c>
-      <c r="C118" s="7">
-        <v>1</v>
-      </c>
-      <c r="D118" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B119" s="11">
-        <v>1</v>
-      </c>
-      <c r="C119" s="7">
-        <v>1</v>
-      </c>
-      <c r="D119" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -2799,7 +2973,7 @@
       <c r="A122" t="s">
         <v>104</v>
       </c>
-      <c r="B122" s="11"/>
+      <c r="B122" s="15"/>
       <c r="C122">
         <v>2</v>
       </c>
@@ -2808,7 +2982,7 @@
       <c r="A123" t="s">
         <v>123</v>
       </c>
-      <c r="B123" s="11"/>
+      <c r="B123" s="15"/>
       <c r="C123">
         <v>1</v>
       </c>
@@ -2817,9 +2991,7 @@
       <c r="A124" t="s">
         <v>120</v>
       </c>
-      <c r="B124" s="11">
-        <v>0</v>
-      </c>
+      <c r="B124" s="15"/>
       <c r="C124">
         <v>2</v>
       </c>
@@ -2828,7 +3000,7 @@
       <c r="A125" t="s">
         <v>121</v>
       </c>
-      <c r="B125" s="11"/>
+      <c r="B125" s="15"/>
       <c r="C125">
         <v>2</v>
       </c>
@@ -2837,7 +3009,7 @@
       <c r="A126" t="s">
         <v>122</v>
       </c>
-      <c r="B126" s="11"/>
+      <c r="B126" s="15"/>
       <c r="C126">
         <v>2</v>
       </c>
@@ -2846,7 +3018,7 @@
       <c r="A127" t="s">
         <v>117</v>
       </c>
-      <c r="B127" s="11"/>
+      <c r="B127" s="15"/>
       <c r="C127">
         <v>2</v>
       </c>
@@ -2869,7 +3041,7 @@
       <c r="A130" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B130" s="11"/>
+      <c r="B130" s="15"/>
       <c r="C130">
         <v>15</v>
       </c>
@@ -2878,24 +3050,22 @@
       <c r="A131" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B131" s="11">
-        <v>2</v>
-      </c>
+      <c r="B131" s="15"/>
       <c r="C131">
         <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>127</v>
-      </c>
-      <c r="B134">
+        <v>126</v>
+      </c>
+      <c r="B134" s="11">
         <f>SUM(B32:B131)</f>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C134">
         <f>B134/(100-8)</f>
-        <v>0.29347826086956524</v>
+        <v>0.32608695652173914</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
log tracability for scenario 2
</commit_message>
<xml_diff>
--- a/Docs/correction_grid.xlsx
+++ b/Docs/correction_grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\Quest\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B0D487-C82E-484F-A4E6-F340589CF86B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB7D3DE-EC6A-4133-854A-A3C31BBE11EE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="160">
   <si>
     <t>is it possible for a participant to NOT play a card for a stage</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -705,6 +705,15 @@
   </si>
   <si>
     <t>s1.log[114-125]</t>
+  </si>
+  <si>
+    <t>s2e.log[9871-9990]</t>
+  </si>
+  <si>
+    <t>s2.log[61-64]</t>
+  </si>
+  <si>
+    <t>s2.log[65-73], s2e.log[12849-13096]</t>
   </si>
 </sst>
 </file>
@@ -1722,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2460,6 +2469,9 @@
       <c r="C69" s="5">
         <v>1</v>
       </c>
+      <c r="D69" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
@@ -2469,6 +2481,9 @@
       <c r="C70" s="5">
         <v>2</v>
       </c>
+      <c r="D70" t="s">
+        <v>158</v>
+      </c>
       <c r="E70" s="5"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2478,6 +2493,9 @@
       <c r="B71" s="15"/>
       <c r="C71" s="5">
         <v>2</v>
+      </c>
+      <c r="D71" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
By Guy: correction grid logs for all other functionality
</commit_message>
<xml_diff>
--- a/Docs/correction_grid.xlsx
+++ b/Docs/correction_grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\Quest\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E45C65-EC77-4203-BEE7-1D4C08FD5998}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC348053-58A5-4A84-94E2-3CA3C8D079C5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="182">
   <si>
     <t>is it possible for a participant to NOT play a card for a stage</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -611,9 +611,6 @@
     <t>use of JSON</t>
   </si>
   <si>
-    <t>tbd</t>
-  </si>
-  <si>
     <t>Claimed Total</t>
   </si>
   <si>
@@ -720,6 +717,69 @@
   </si>
   <si>
     <t>s1e.log</t>
+  </si>
+  <si>
+    <t>aimatch.log[486-489]</t>
+  </si>
+  <si>
+    <t>aimatch.log[888-890]</t>
+  </si>
+  <si>
+    <t>aimatch.log[663-671]</t>
+  </si>
+  <si>
+    <t>aimatch.log[145-148]</t>
+  </si>
+  <si>
+    <t>aimatch.log[10-57]</t>
+  </si>
+  <si>
+    <t>addai.log[1-34]</t>
+  </si>
+  <si>
+    <t>addai.log[1-34], unsure if tests are a requirement</t>
+  </si>
+  <si>
+    <t>test1.log[66-99]</t>
+  </si>
+  <si>
+    <t>test2.log[2194-2195]</t>
+  </si>
+  <si>
+    <t>test3.log[54-66]</t>
+  </si>
+  <si>
+    <t>test4.log[76-80]</t>
+  </si>
+  <si>
+    <t>test4.log[54-68]</t>
+  </si>
+  <si>
+    <t>test4.log[70-73]</t>
+  </si>
+  <si>
+    <t>test5.log[63-65]</t>
+  </si>
+  <si>
+    <t>test6.log[50-62]</t>
+  </si>
+  <si>
+    <t>test7.log[54-68]</t>
+  </si>
+  <si>
+    <t>Special features</t>
+  </si>
+  <si>
+    <t>Can be run in browser and as a desktop application.</t>
+  </si>
+  <si>
+    <t>aimatch.log[60]</t>
+  </si>
+  <si>
+    <t>test8.log(88-117)</t>
+  </si>
+  <si>
+    <t>aimatch.log[91-97]</t>
   </si>
 </sst>
 </file>
@@ -1735,10 +1795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F134"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1943,7 +2003,7 @@
         <v>5</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1966,7 +2026,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2030,7 +2090,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2044,7 +2104,7 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2058,7 +2118,7 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2072,7 +2132,7 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2086,7 +2146,7 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2100,7 +2160,7 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2114,7 +2174,7 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2134,7 +2194,7 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2155,7 +2215,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2169,7 +2229,7 @@
         <v>1</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2183,7 +2243,7 @@
         <v>1</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2197,7 +2257,7 @@
         <v>1</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2211,7 +2271,7 @@
         <v>1</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2225,7 +2285,7 @@
         <v>1</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2239,7 +2299,7 @@
         <v>2</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2259,7 +2319,7 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2284,7 +2344,7 @@
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2298,7 +2358,7 @@
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2312,7 +2372,7 @@
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2326,7 +2386,7 @@
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2340,7 +2400,7 @@
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2354,7 +2414,7 @@
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2368,7 +2428,7 @@
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2388,7 +2448,7 @@
         <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2402,7 +2462,7 @@
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2416,7 +2476,7 @@
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2430,7 +2490,7 @@
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2444,7 +2504,7 @@
         <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2478,7 +2538,7 @@
         <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2492,7 +2552,7 @@
         <v>2</v>
       </c>
       <c r="D70" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E70" s="5"/>
     </row>
@@ -2507,7 +2567,7 @@
         <v>2</v>
       </c>
       <c r="D71" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2666,9 +2726,14 @@
       <c r="A88" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B88" s="15"/>
+      <c r="B88" s="15">
+        <v>1</v>
+      </c>
       <c r="C88" s="5">
         <v>1</v>
+      </c>
+      <c r="D88" t="s">
+        <v>165</v>
       </c>
       <c r="E88" s="5"/>
     </row>
@@ -2676,9 +2741,14 @@
       <c r="A89" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B89" s="15"/>
+      <c r="B89" s="15">
+        <v>1</v>
+      </c>
       <c r="C89" s="5">
         <v>1</v>
+      </c>
+      <c r="D89" t="s">
+        <v>179</v>
       </c>
       <c r="E89" s="5"/>
     </row>
@@ -2686,9 +2756,14 @@
       <c r="A90" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B90" s="15"/>
+      <c r="B90" s="15">
+        <v>1</v>
+      </c>
       <c r="C90" s="5">
         <v>1</v>
+      </c>
+      <c r="D90" t="s">
+        <v>181</v>
       </c>
       <c r="E90" s="5"/>
     </row>
@@ -2696,7 +2771,9 @@
       <c r="A91" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B91" s="15"/>
+      <c r="B91" s="15">
+        <v>0</v>
+      </c>
       <c r="C91" s="5">
         <v>1</v>
       </c>
@@ -2724,6 +2801,9 @@
       <c r="C93">
         <v>0.5</v>
       </c>
+      <c r="D93" t="s">
+        <v>180</v>
+      </c>
       <c r="E93" s="5"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2736,6 +2816,9 @@
       <c r="C94">
         <v>0.5</v>
       </c>
+      <c r="D94" t="s">
+        <v>173</v>
+      </c>
       <c r="E94" s="5"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2748,6 +2831,9 @@
       <c r="C95">
         <v>0.5</v>
       </c>
+      <c r="D95" t="s">
+        <v>173</v>
+      </c>
       <c r="E95" s="5"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2760,6 +2846,9 @@
       <c r="C96" s="5">
         <v>0.5</v>
       </c>
+      <c r="D96" t="s">
+        <v>176</v>
+      </c>
       <c r="E96" s="5"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2773,7 +2862,7 @@
         <v>0.5</v>
       </c>
       <c r="D97" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2787,7 +2876,7 @@
         <v>0.5</v>
       </c>
       <c r="D98" t="s">
-        <v>125</v>
+        <v>171</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2801,7 +2890,7 @@
         <v>1</v>
       </c>
       <c r="D99" t="s">
-        <v>125</v>
+        <v>167</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2837,7 +2926,7 @@
         <v>1</v>
       </c>
       <c r="D102" t="s">
-        <v>125</v>
+        <v>168</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2851,7 +2940,7 @@
         <v>1</v>
       </c>
       <c r="D103" t="s">
-        <v>125</v>
+        <v>170</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2876,7 +2965,7 @@
         <v>1</v>
       </c>
       <c r="D105" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2890,7 +2979,7 @@
         <v>0.5</v>
       </c>
       <c r="D106" t="s">
-        <v>125</v>
+        <v>174</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2938,7 +3027,7 @@
         <v>1</v>
       </c>
       <c r="D110" t="s">
-        <v>125</v>
+        <v>175</v>
       </c>
       <c r="E110" s="5"/>
     </row>
@@ -2953,7 +3042,7 @@
         <v>0.5</v>
       </c>
       <c r="D111" t="s">
-        <v>125</v>
+        <v>169</v>
       </c>
       <c r="E111" s="5"/>
     </row>
@@ -2992,7 +3081,7 @@
         <v>1</v>
       </c>
       <c r="D114" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="E114" s="5"/>
     </row>
@@ -3007,7 +3096,7 @@
         <v>1</v>
       </c>
       <c r="D115" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3043,7 +3132,7 @@
         <v>1</v>
       </c>
       <c r="D118" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3057,7 +3146,7 @@
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3165,7 +3254,7 @@
         <v>15</v>
       </c>
       <c r="D130" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3179,20 +3268,30 @@
         <v>2</v>
       </c>
       <c r="D131" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B134" s="11">
         <f>SUM(B32:B131)</f>
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C134">
         <f>B134/(100-8)</f>
-        <v>0.70652173913043481</v>
+        <v>0.73913043478260865</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>